<commit_message>
update data of meta and others
</commit_message>
<xml_diff>
--- a/data/echoMRI/kotz03102025.xlsx
+++ b/data/echoMRI/kotz03102025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B81EAF4-8264-B249-9F35-44E32BB4C8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B30902-F3B7-D841-BE86-4ACA8195750C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="22780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedScans" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>RecNumber</t>
   </si>
@@ -53,15 +53,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>1002</t>
-  </si>
-  <si>
-    <t>1003</t>
   </si>
   <si>
     <t>8098</t>
@@ -448,7 +439,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -492,8 +483,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2">
+        <v>8097</v>
       </c>
       <c r="C2">
         <v>1.45</v>
@@ -508,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -521,8 +512,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
+      <c r="B3">
+        <v>8096</v>
       </c>
       <c r="C3">
         <v>1.25</v>
@@ -537,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -550,8 +541,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4">
+        <v>8095</v>
       </c>
       <c r="C4">
         <v>1.31</v>
@@ -566,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -580,7 +571,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1.3</v>
@@ -595,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -609,7 +600,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1.3</v>
@@ -624,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -638,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>1.25</v>
@@ -653,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -667,7 +658,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>1.82</v>
@@ -682,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -696,7 +687,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>0.85</v>
@@ -711,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -725,7 +716,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>1.1399999999999999</v>
@@ -740,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H10">
         <v>1</v>

</xml_diff>